<commit_message>
firewall spreadsheet add logo
</commit_message>
<xml_diff>
--- a/firewall-rules.xlsx
+++ b/firewall-rules.xlsx
@@ -222,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -247,6 +247,7 @@
     <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,10 +265,53 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114632</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="165100" y="0"/>
+          <a:ext cx="5803900" cy="1270332"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Blue Warm">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -275,34 +319,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="242852"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="ACCBF9"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4A66AC"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="629DD1"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="297FD5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="7F8FA9"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5AA2AE"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="9D90A0"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="9454C3"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="3EBBF0"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -636,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H21"/>
+  <dimension ref="B10:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -654,352 +698,355 @@
     <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:8" s="3" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="2:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="2:8" s="3" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
+    <row r="13" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G13" s="9">
         <v>80443</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
+    <row r="14" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G14" s="9">
         <v>22446</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H14" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+    <row r="15" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G15" s="8">
         <v>1521</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+    <row r="16" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G16" s="8">
         <v>8080</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H16" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+    <row r="17" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G17" s="8">
         <v>443</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H17" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+    <row r="18" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G18" s="8">
         <v>443</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H18" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
+    <row r="19" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G19" s="9">
         <v>22446</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H19" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="7" t="s">
+    <row r="20" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B19" s="6"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="H21" s="2"/>
     </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B28" s="6"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B29" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Destination" prompt="Please enter the destination IP(s)._x000a_For incoming rules, this will be the IP(s) of your server(s)._x000a_For outgoing rules, this will be the IP(s) that connections will be made to._x000a_Use 'ANY' to specify the entire internet for outgoing rules" sqref="B11:C11 C12:C21 C3:C10">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Destination" prompt="Please enter the destination IP(s)._x000a_For incoming rules, this will be the IP(s) of your server(s)._x000a_For outgoing rules, this will be the IP(s) that connections will be made to._x000a_Use 'ANY' to specify the entire internet for outgoing rules" sqref="B20:C20 C21:C30 C12:C19">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source" prompt="Please enter the originating IP in this entry._x000a_For outgoing rules, this will be the IP(s) of your server(s)._x000a_For incoming rules, this will be the IP(s) that connections will be originating from._x000a_Use 'ANY' to specify the entire internet for incoming rules." sqref="B3:B10 B12:B21">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source" prompt="Please enter the originating IP in this entry._x000a_For outgoing rules, this will be the IP(s) of your server(s)._x000a_For incoming rules, this will be the IP(s) that connections will be originating from._x000a_Use 'ANY' to specify the entire internet for incoming rules." sqref="B12:B19 B21:B30">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Protocol" prompt="Specify the protocol here. _x000a_Most commonly your protocol will be either TCP or UDP unless you have very specific requirements" sqref="D3:D21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Protocol" prompt="Specify the protocol here. _x000a_Most commonly your protocol will be either TCP or UDP unless you have very specific requirements" sqref="D12:D30">
       <formula1>proto</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Direction" prompt="The direction of your rule. Select 'IN' for incoming rules and 'OUT-INSIDE' for ougoing rules." sqref="E3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Direction" prompt="The direction of your rule. Select 'IN' for incoming rules and 'OUT-INSIDE' for ougoing rules." sqref="E12">
       <formula1>direction</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Action" prompt="Select whether to 'ALLOW' or 'DENY' traffic" sqref="F3:F21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Action" prompt="Select whether to 'ALLOW' or 'DENY' traffic" sqref="F12:F30">
       <formula1>rule</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Ports" prompt="Use comma separated numerical values to specify individual ports._x000a_Use a '-' to specify a range of ports._x000a_Specify 'ANY' to allow all ports." sqref="G3:G21">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Ports" prompt="Use comma separated numerical values to specify individual ports._x000a_Use a '-' to specify a range of ports._x000a_Specify 'ANY' to allow all ports." sqref="G12:G30">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Notes" prompt="Any additional information for this rule" sqref="H3:H21">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Notes" prompt="Any additional information for this rule" sqref="H12:H30">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Direction" prompt="The direction of your rule. Select 'IN' for incoming rules and 'OUT' for ougoing rules." sqref="E4:E21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Direction" prompt="The direction of your rule. Select 'IN' for incoming rules and 'OUT' for ougoing rules." sqref="E13:E30">
       <formula1>direction</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D7">
       <formula1>proto</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E7">
       <formula1>direction</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F7">
       <formula1>rule</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1007,6 +1054,7 @@
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>